<commit_message>
Resolve incorrect date format
</commit_message>
<xml_diff>
--- a/src/out.xlsx
+++ b/src/out.xlsx
@@ -466,7 +466,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27883</v>
       </c>
       <c r="B2" t="n">
         <v>482</v>
@@ -478,12 +478,12 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27914</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27884</v>
       </c>
       <c r="B3" t="n">
         <v>484</v>
@@ -495,12 +495,12 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27915</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27885</v>
       </c>
       <c r="B4" t="n">
         <v>489.25</v>
@@ -512,12 +512,12 @@
         <v>5.25</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27916</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27886</v>
       </c>
       <c r="B5" t="n">
         <v>490.5</v>
@@ -529,12 +529,12 @@
         <v>4.5</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27917</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27887</v>
       </c>
       <c r="B6" t="n">
         <v>501.75</v>
@@ -546,12 +546,12 @@
         <v>8.75</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27918</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27890</v>
       </c>
       <c r="B7" t="n">
         <v>509.5</v>
@@ -563,12 +563,12 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27921</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27891</v>
       </c>
       <c r="B8" t="n">
         <v>511.5</v>
@@ -580,12 +580,12 @@
         <v>8.25</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27922</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27892</v>
       </c>
       <c r="B9" t="n">
         <v>517</v>
@@ -597,12 +597,12 @@
         <v>7.5</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27923</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27893</v>
       </c>
       <c r="B10" t="n">
         <v>515</v>
@@ -614,12 +614,12 @@
         <v>7</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27924</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27894</v>
       </c>
       <c r="B11" t="n">
         <v>523</v>
@@ -631,12 +631,12 @@
         <v>5.5</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27925</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27897</v>
       </c>
       <c r="B12" t="n">
         <v>536.5</v>
@@ -648,12 +648,12 @@
         <v>14.5</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27928</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27898</v>
       </c>
       <c r="B13" t="n">
         <v>534</v>
@@ -665,12 +665,12 @@
         <v>9</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27929</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27899</v>
       </c>
       <c r="B14" t="n">
         <v>530</v>
@@ -682,12 +682,12 @@
         <v>7</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27930</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27900</v>
       </c>
       <c r="B15" t="n">
         <v>550.5</v>
@@ -699,12 +699,12 @@
         <v>12</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27931</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27901</v>
       </c>
       <c r="B16" t="n">
         <v>548</v>
@@ -716,12 +716,12 @@
         <v>9</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27932</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27904</v>
       </c>
       <c r="B17" t="n">
         <v>567.5</v>
@@ -733,12 +733,12 @@
         <v>17.5</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27935</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27905</v>
       </c>
       <c r="B18" t="n">
         <v>575</v>
@@ -750,12 +750,12 @@
         <v>18</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27936</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27906</v>
       </c>
       <c r="B19" t="n">
         <v>578</v>
@@ -767,12 +767,12 @@
         <v>17</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27937</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27907</v>
       </c>
       <c r="B20" t="n">
         <v>587</v>
@@ -784,12 +784,12 @@
         <v>16.5</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27938</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27908</v>
       </c>
       <c r="B21" t="n">
         <v>581</v>
@@ -801,12 +801,12 @@
         <v>14.25</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27939</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27912</v>
       </c>
       <c r="B22" t="n">
         <v>597</v>
@@ -818,12 +818,12 @@
         <v>24</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27942</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27913</v>
       </c>
       <c r="B23" t="n">
         <v>598</v>
@@ -835,12 +835,12 @@
         <v>14</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27943</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27914</v>
       </c>
       <c r="B24" t="n">
         <v>590.25</v>
@@ -852,12 +852,12 @@
         <v>11.25</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27944</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27915</v>
       </c>
       <c r="B25" t="n">
         <v>587.5</v>
@@ -869,12 +869,12 @@
         <v>10.5</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27945</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27918</v>
       </c>
       <c r="B26" t="n">
         <v>603.5</v>
@@ -886,12 +886,12 @@
         <v>11.5</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27948</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27919</v>
       </c>
       <c r="B27" t="n">
         <v>623.5</v>
@@ -903,12 +903,12 @@
         <v>12.5</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27949</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27920</v>
       </c>
       <c r="B28" t="n">
         <v>633</v>
@@ -920,12 +920,12 @@
         <v>12.5</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27950</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27921</v>
       </c>
       <c r="B29" t="n">
         <v>647.75</v>
@@ -937,12 +937,12 @@
         <v>6.75</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27951</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27922</v>
       </c>
       <c r="B30" t="n">
         <v>667</v>
@@ -954,12 +954,12 @@
         <v>25</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27952</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27925</v>
       </c>
       <c r="B31" t="n">
         <v>680</v>
@@ -971,12 +971,12 @@
         <v>18</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27955</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27926</v>
       </c>
       <c r="B32" t="n">
         <v>680</v>
@@ -988,12 +988,12 @@
         <v>21.5</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27956</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27927</v>
       </c>
       <c r="B33" t="n">
         <v>661</v>
@@ -1005,12 +1005,12 @@
         <v>19</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27957</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27928</v>
       </c>
       <c r="B34" t="n">
         <v>654</v>
@@ -1022,12 +1022,12 @@
         <v>30.5</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27958</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27929</v>
       </c>
       <c r="B35" t="n">
         <v>627.25</v>
@@ -1039,12 +1039,12 @@
         <v>14.25</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27959</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27932</v>
       </c>
       <c r="B36" t="n">
         <v>636.5</v>
@@ -1056,12 +1056,12 @@
         <v>20.5</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27962</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27933</v>
       </c>
       <c r="B37" t="n">
         <v>656.5</v>
@@ -1073,12 +1073,12 @@
         <v>13.5</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27963</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27934</v>
       </c>
       <c r="B38" t="n">
         <v>645</v>
@@ -1090,12 +1090,12 @@
         <v>9.75</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27964</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27935</v>
       </c>
       <c r="B39" t="n">
         <v>655.25</v>
@@ -1107,12 +1107,12 @@
         <v>27.75</v>
       </c>
       <c r="E39" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27965</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27936</v>
       </c>
       <c r="B40" t="n">
         <v>672</v>
@@ -1124,12 +1124,12 @@
         <v>14</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27966</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27939</v>
       </c>
       <c r="B41" t="n">
         <v>674</v>
@@ -1141,12 +1141,12 @@
         <v>14</v>
       </c>
       <c r="E41" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27969</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27940</v>
       </c>
       <c r="B42" t="n">
         <v>672</v>
@@ -1158,12 +1158,12 @@
         <v>11</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27970</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27941</v>
       </c>
       <c r="B43" t="n">
         <v>677</v>
@@ -1175,12 +1175,12 @@
         <v>19</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27971</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27942</v>
       </c>
       <c r="B44" t="n">
         <v>687</v>
@@ -1192,12 +1192,12 @@
         <v>25</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27973</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27943</v>
       </c>
       <c r="B45" t="n">
         <v>707</v>
@@ -1209,12 +1209,12 @@
         <v>0</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27974</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27947</v>
       </c>
       <c r="B46" t="n">
         <v>727</v>
@@ -1226,12 +1226,12 @@
         <v>0</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27978</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27948</v>
       </c>
       <c r="B47" t="n">
         <v>757</v>
@@ -1243,12 +1243,12 @@
         <v>52</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27979</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27949</v>
       </c>
       <c r="B48" t="n">
         <v>733.88</v>
@@ -1260,12 +1260,12 @@
         <v>29.88</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27980</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27950</v>
       </c>
       <c r="B49" t="n">
         <v>750</v>
@@ -1277,12 +1277,12 @@
         <v>15</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27981</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27953</v>
       </c>
       <c r="B50" t="n">
         <v>751</v>
@@ -1294,12 +1294,12 @@
         <v>26.5</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27984</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27954</v>
       </c>
       <c r="B51" t="n">
         <v>729</v>
@@ -1311,12 +1311,12 @@
         <v>19</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27985</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27955</v>
       </c>
       <c r="B52" t="n">
         <v>733.5</v>
@@ -1328,12 +1328,12 @@
         <v>16.5</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27986</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27956</v>
       </c>
       <c r="B53" t="n">
         <v>743</v>
@@ -1345,12 +1345,12 @@
         <v>29.5</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27987</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27957</v>
       </c>
       <c r="B54" t="n">
         <v>715</v>
@@ -1362,12 +1362,12 @@
         <v>18</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27988</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27960</v>
       </c>
       <c r="B55" t="n">
         <v>704</v>
@@ -1379,12 +1379,12 @@
         <v>23</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27991</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27961</v>
       </c>
       <c r="B56" t="n">
         <v>673</v>
@@ -1396,12 +1396,12 @@
         <v>12</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27992</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27962</v>
       </c>
       <c r="B57" t="n">
         <v>670</v>
@@ -1413,12 +1413,12 @@
         <v>15</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27993</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27963</v>
       </c>
       <c r="B58" t="n">
         <v>657</v>
@@ -1430,12 +1430,12 @@
         <v>14.5</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27994</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27964</v>
       </c>
       <c r="B59" t="n">
         <v>662</v>
@@ -1447,12 +1447,12 @@
         <v>39.5</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27995</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27967</v>
       </c>
       <c r="B60" t="n">
         <v>654</v>
@@ -1464,12 +1464,12 @@
         <v>13.5</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27998</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27968</v>
       </c>
       <c r="B61" t="n">
         <v>637</v>
@@ -1481,12 +1481,12 @@
         <v>16.5</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>27999</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27969</v>
       </c>
       <c r="B62" t="n">
         <v>638.5</v>
@@ -1498,12 +1498,12 @@
         <v>14.5</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28000</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27970</v>
       </c>
       <c r="B63" t="n">
         <v>633</v>
@@ -1515,12 +1515,12 @@
         <v>16.25</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28001</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27971</v>
       </c>
       <c r="B64" t="n">
         <v>631</v>
@@ -1532,12 +1532,12 @@
         <v>28.75</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28002</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27974</v>
       </c>
       <c r="B65" t="n">
         <v>609</v>
@@ -1549,12 +1549,12 @@
         <v>23.5</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28005</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27975</v>
       </c>
       <c r="B66" t="n">
         <v>601</v>
@@ -1566,12 +1566,12 @@
         <v>24</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28006</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27976</v>
       </c>
       <c r="B67" t="n">
         <v>616</v>
@@ -1583,12 +1583,12 @@
         <v>10</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28007</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27977</v>
       </c>
       <c r="B68" t="n">
         <v>626</v>
@@ -1600,12 +1600,12 @@
         <v>16</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28008</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27978</v>
       </c>
       <c r="B69" t="n">
         <v>624</v>
@@ -1617,12 +1617,12 @@
         <v>12</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28009</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27981</v>
       </c>
       <c r="B70" t="n">
         <v>633</v>
@@ -1634,12 +1634,12 @@
         <v>15</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28012</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27982</v>
       </c>
       <c r="B71" t="n">
         <v>627.5</v>
@@ -1651,12 +1651,12 @@
         <v>13.5</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28013</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27983</v>
       </c>
       <c r="B72" t="n">
         <v>616</v>
@@ -1668,12 +1668,12 @@
         <v>4</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28014</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27984</v>
       </c>
       <c r="B73" t="n">
         <v>629</v>
@@ -1685,12 +1685,12 @@
         <v>10</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28015</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27985</v>
       </c>
       <c r="B74" t="n">
         <v>648</v>
@@ -1702,12 +1702,12 @@
         <v>21</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28016</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27988</v>
       </c>
       <c r="B75" t="n">
         <v>648</v>
@@ -1719,12 +1719,12 @@
         <v>8</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28019</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27989</v>
       </c>
       <c r="B76" t="n">
         <v>639</v>
@@ -1736,12 +1736,12 @@
         <v>17.5</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28020</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27990</v>
       </c>
       <c r="B77" t="n">
         <v>632</v>
@@ -1753,12 +1753,12 @@
         <v>15</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28021</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27991</v>
       </c>
       <c r="B78" t="n">
         <v>648</v>
@@ -1770,12 +1770,12 @@
         <v>4</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28022</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27992</v>
       </c>
       <c r="B79" t="n">
         <v>666</v>
@@ -1787,12 +1787,12 @@
         <v>9</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28023</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27995</v>
       </c>
       <c r="B80" t="n">
         <v>679.5</v>
@@ -1804,12 +1804,12 @@
         <v>7.5</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28026</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27996</v>
       </c>
       <c r="B81" t="n">
         <v>686</v>
@@ -1821,12 +1821,12 @@
         <v>23</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28027</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27997</v>
       </c>
       <c r="B82" t="n">
         <v>675.5</v>
@@ -1838,12 +1838,12 @@
         <v>17.5</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28028</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27998</v>
       </c>
       <c r="B83" t="n">
         <v>678</v>
@@ -1855,12 +1855,12 @@
         <v>26</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28029</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>27999</v>
       </c>
       <c r="B84" t="n">
         <v>688</v>
@@ -1872,12 +1872,12 @@
         <v>15</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28030</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28002</v>
       </c>
       <c r="B85" t="n">
         <v>688.5</v>
@@ -1889,12 +1889,12 @@
         <v>21.5</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28033</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28003</v>
       </c>
       <c r="B86" t="n">
         <v>677</v>
@@ -1906,12 +1906,12 @@
         <v>14</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28033</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28004</v>
       </c>
       <c r="B87" t="n">
         <v>682</v>
@@ -1923,12 +1923,12 @@
         <v>19.5</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28034</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28005</v>
       </c>
       <c r="B88" t="n">
         <v>699.5</v>
@@ -1940,12 +1940,12 @@
         <v>9.5</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28035</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28006</v>
       </c>
       <c r="B89" t="n">
         <v>712</v>
@@ -1957,12 +1957,12 @@
         <v>18</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28036</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28010</v>
       </c>
       <c r="B90" t="n">
         <v>730</v>
@@ -1974,12 +1974,12 @@
         <v>0</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28040</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28011</v>
       </c>
       <c r="B91" t="n">
         <v>746</v>
@@ -1991,12 +1991,12 @@
         <v>26</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28041</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28012</v>
       </c>
       <c r="B92" t="n">
         <v>736.5</v>
@@ -2008,12 +2008,12 @@
         <v>17.5</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28042</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28013</v>
       </c>
       <c r="B93" t="n">
         <v>740</v>
@@ -2025,12 +2025,12 @@
         <v>12</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28043</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28016</v>
       </c>
       <c r="B94" t="n">
         <v>725</v>
@@ -2042,12 +2042,12 @@
         <v>16.5</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28046</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28017</v>
       </c>
       <c r="B95" t="n">
         <v>709.5</v>
@@ -2059,12 +2059,12 @@
         <v>21</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28047</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28018</v>
       </c>
       <c r="B96" t="n">
         <v>693</v>
@@ -2076,12 +2076,12 @@
         <v>21</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28048</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28019</v>
       </c>
       <c r="B97" t="n">
         <v>692</v>
@@ -2093,12 +2093,12 @@
         <v>9.5</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28049</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28020</v>
       </c>
       <c r="B98" t="n">
         <v>676</v>
@@ -2110,12 +2110,12 @@
         <v>13</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28050</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28023</v>
       </c>
       <c r="B99" t="n">
         <v>652</v>
@@ -2127,12 +2127,12 @@
         <v>9</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28053</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28024</v>
       </c>
       <c r="B100" t="n">
         <v>657</v>
@@ -2144,12 +2144,12 @@
         <v>6</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28054</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28025</v>
       </c>
       <c r="B101" t="n">
         <v>652.5</v>
@@ -2161,12 +2161,12 @@
         <v>12.5</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28055</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28026</v>
       </c>
       <c r="B102" t="n">
         <v>660</v>
@@ -2178,12 +2178,12 @@
         <v>30</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28056</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28027</v>
       </c>
       <c r="B103" t="n">
         <v>656.5</v>
@@ -2195,12 +2195,12 @@
         <v>16.5</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28057</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28030</v>
       </c>
       <c r="B104" t="n">
         <v>645</v>
@@ -2212,12 +2212,12 @@
         <v>20</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28060</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28031</v>
       </c>
       <c r="B105" t="n">
         <v>644</v>
@@ -2229,12 +2229,12 @@
         <v>13.5</v>
       </c>
       <c r="E105" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28061</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28032</v>
       </c>
       <c r="B106" t="n">
         <v>639.5</v>
@@ -2246,12 +2246,12 @@
         <v>18.5</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28062</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>25569.00000022871</v>
+        <v>28033</v>
       </c>
       <c r="B107" t="n">
         <v>633</v>
@@ -2263,12 +2263,12 @@
         <v>19</v>
       </c>
       <c r="E107" s="2" t="n">
-        <v>25600.00000022871</v>
+        <v>28063</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28034</v>
       </c>
       <c r="B108" t="n">
         <v>633.5</v>
@@ -2280,12 +2280,12 @@
         <v>14.5</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28065</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28037</v>
       </c>
       <c r="B109" t="n">
         <v>640</v>
@@ -2297,12 +2297,12 @@
         <v>26</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28068</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28038</v>
       </c>
       <c r="B110" t="n">
         <v>660</v>
@@ -2314,12 +2314,12 @@
         <v>26</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28069</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28039</v>
       </c>
       <c r="B111" t="n">
         <v>662</v>
@@ -2331,12 +2331,12 @@
         <v>20</v>
       </c>
       <c r="E111" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28070</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28040</v>
       </c>
       <c r="B112" t="n">
         <v>662.5</v>
@@ -2348,12 +2348,12 @@
         <v>11.5</v>
       </c>
       <c r="E112" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28071</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28041</v>
       </c>
       <c r="B113" t="n">
         <v>665</v>
@@ -2365,12 +2365,12 @@
         <v>18</v>
       </c>
       <c r="E113" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28072</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28044</v>
       </c>
       <c r="B114" t="n">
         <v>654</v>
@@ -2382,12 +2382,12 @@
         <v>20.5</v>
       </c>
       <c r="E114" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28075</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28045</v>
       </c>
       <c r="B115" t="n">
         <v>636</v>
@@ -2399,12 +2399,12 @@
         <v>12</v>
       </c>
       <c r="E115" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28076</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28046</v>
       </c>
       <c r="B116" t="n">
         <v>645.5</v>
@@ -2416,12 +2416,12 @@
         <v>0</v>
       </c>
       <c r="E116" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28077</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28047</v>
       </c>
       <c r="B117" t="n">
         <v>660</v>
@@ -2433,12 +2433,12 @@
         <v>34.25</v>
       </c>
       <c r="E117" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28078</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28048</v>
       </c>
       <c r="B118" t="n">
         <v>633</v>
@@ -2450,12 +2450,12 @@
         <v>15</v>
       </c>
       <c r="E118" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28079</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28051</v>
       </c>
       <c r="B119" t="n">
         <v>628</v>
@@ -2467,12 +2467,12 @@
         <v>24</v>
       </c>
       <c r="E119" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28082</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28052</v>
       </c>
       <c r="B120" t="n">
         <v>625</v>
@@ -2484,12 +2484,12 @@
         <v>15</v>
       </c>
       <c r="E120" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28083</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28053</v>
       </c>
       <c r="B121" t="n">
         <v>625</v>
@@ -2501,12 +2501,12 @@
         <v>8.5</v>
       </c>
       <c r="E121" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28084</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28054</v>
       </c>
       <c r="B122" t="n">
         <v>633</v>
@@ -2518,12 +2518,12 @@
         <v>11</v>
       </c>
       <c r="E122" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28085</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28055</v>
       </c>
       <c r="B123" t="n">
         <v>653</v>
@@ -2535,12 +2535,12 @@
         <v>31.5</v>
       </c>
       <c r="E123" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28086</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28058</v>
       </c>
       <c r="B124" t="n">
         <v>662</v>
@@ -2552,12 +2552,12 @@
         <v>19</v>
       </c>
       <c r="E124" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28089</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28059</v>
       </c>
       <c r="B125" t="n">
         <v>663.5</v>
@@ -2569,12 +2569,12 @@
         <v>19.5</v>
       </c>
       <c r="E125" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28090</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28060</v>
       </c>
       <c r="B126" t="n">
         <v>673</v>
@@ -2586,12 +2586,12 @@
         <v>25</v>
       </c>
       <c r="E126" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28091</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28061</v>
       </c>
       <c r="B127" t="n">
         <v>672</v>
@@ -2603,12 +2603,12 @@
         <v>16</v>
       </c>
       <c r="E127" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28092</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28062</v>
       </c>
       <c r="B128" t="n">
         <v>679</v>
@@ -2620,12 +2620,12 @@
         <v>28</v>
       </c>
       <c r="E128" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28093</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28065</v>
       </c>
       <c r="B129" t="n">
         <v>680</v>
@@ -2637,12 +2637,12 @@
         <v>11</v>
       </c>
       <c r="E129" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28095</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28067</v>
       </c>
       <c r="B130" t="n">
         <v>676</v>
@@ -2654,12 +2654,12 @@
         <v>27</v>
       </c>
       <c r="E130" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28097</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28068</v>
       </c>
       <c r="B131" t="n">
         <v>670</v>
@@ -2671,12 +2671,12 @@
         <v>20</v>
       </c>
       <c r="E131" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28098</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28069</v>
       </c>
       <c r="B132" t="n">
         <v>672</v>
@@ -2688,12 +2688,12 @@
         <v>13</v>
       </c>
       <c r="E132" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28099</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28072</v>
       </c>
       <c r="B133" t="n">
         <v>678</v>
@@ -2705,12 +2705,12 @@
         <v>14</v>
       </c>
       <c r="E133" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28102</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28073</v>
       </c>
       <c r="B134" t="n">
         <v>666</v>
@@ -2722,12 +2722,12 @@
         <v>12.5</v>
       </c>
       <c r="E134" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28103</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28074</v>
       </c>
       <c r="B135" t="n">
         <v>670</v>
@@ -2739,12 +2739,12 @@
         <v>10.5</v>
       </c>
       <c r="E135" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28104</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28075</v>
       </c>
       <c r="B136" t="n">
         <v>657</v>
@@ -2756,12 +2756,12 @@
         <v>17</v>
       </c>
       <c r="E136" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28105</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28076</v>
       </c>
       <c r="B137" t="n">
         <v>654</v>
@@ -2773,12 +2773,12 @@
         <v>7</v>
       </c>
       <c r="E137" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28106</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28079</v>
       </c>
       <c r="B138" t="n">
         <v>647</v>
@@ -2790,12 +2790,12 @@
         <v>22.5</v>
       </c>
       <c r="E138" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28109</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28080</v>
       </c>
       <c r="B139" t="n">
         <v>650.5</v>
@@ -2807,12 +2807,12 @@
         <v>18.5</v>
       </c>
       <c r="E139" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28110</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28081</v>
       </c>
       <c r="B140" t="n">
         <v>671</v>
@@ -2824,12 +2824,12 @@
         <v>25</v>
       </c>
       <c r="E140" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28111</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28082</v>
       </c>
       <c r="B141" t="n">
         <v>676</v>
@@ -2841,12 +2841,12 @@
         <v>17</v>
       </c>
       <c r="E141" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28112</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28083</v>
       </c>
       <c r="B142" t="n">
         <v>691</v>
@@ -2858,12 +2858,12 @@
         <v>21.5</v>
       </c>
       <c r="E142" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28113</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28086</v>
       </c>
       <c r="B143" t="n">
         <v>691</v>
@@ -2875,12 +2875,12 @@
         <v>16.5</v>
       </c>
       <c r="E143" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28116</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28087</v>
       </c>
       <c r="B144" t="n">
         <v>696.5</v>
@@ -2892,12 +2892,12 @@
         <v>22</v>
       </c>
       <c r="E144" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28117</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28088</v>
       </c>
       <c r="B145" t="n">
         <v>686</v>
@@ -2909,12 +2909,12 @@
         <v>7.5</v>
       </c>
       <c r="E145" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28118</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28090</v>
       </c>
       <c r="B146" t="n">
         <v>681.5</v>
@@ -2926,12 +2926,12 @@
         <v>11</v>
       </c>
       <c r="E146" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28120</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28093</v>
       </c>
       <c r="B147" t="n">
         <v>675</v>
@@ -2943,12 +2943,12 @@
         <v>13.5</v>
       </c>
       <c r="E147" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28123</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28094</v>
       </c>
       <c r="B148" t="n">
         <v>677.5</v>
@@ -2960,12 +2960,12 @@
         <v>11.5</v>
       </c>
       <c r="E148" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28124</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28095</v>
       </c>
       <c r="B149" t="n">
         <v>681.5</v>
@@ -2977,12 +2977,12 @@
         <v>8.5</v>
       </c>
       <c r="E149" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28126</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28096</v>
       </c>
       <c r="B150" t="n">
         <v>681.5</v>
@@ -2994,12 +2994,12 @@
         <v>6.5</v>
       </c>
       <c r="E150" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28127</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28097</v>
       </c>
       <c r="B151" t="n">
         <v>687</v>
@@ -3011,12 +3011,12 @@
         <v>8</v>
       </c>
       <c r="E151" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28128</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28100</v>
       </c>
       <c r="B152" t="n">
         <v>698.5</v>
@@ -3028,12 +3028,12 @@
         <v>9.5</v>
       </c>
       <c r="E152" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28131</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28101</v>
       </c>
       <c r="B153" t="n">
         <v>700</v>
@@ -3045,12 +3045,12 @@
         <v>10</v>
       </c>
       <c r="E153" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28132</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28102</v>
       </c>
       <c r="B154" t="n">
         <v>708</v>
@@ -3062,12 +3062,12 @@
         <v>17</v>
       </c>
       <c r="E154" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28133</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28103</v>
       </c>
       <c r="B155" t="n">
         <v>712</v>
@@ -3079,12 +3079,12 @@
         <v>10</v>
       </c>
       <c r="E155" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28134</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28104</v>
       </c>
       <c r="B156" t="n">
         <v>704</v>
@@ -3096,12 +3096,12 @@
         <v>8</v>
       </c>
       <c r="E156" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28135</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28107</v>
       </c>
       <c r="B157" t="n">
         <v>695</v>
@@ -3113,12 +3113,12 @@
         <v>4.5</v>
       </c>
       <c r="E157" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28138</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28108</v>
       </c>
       <c r="B158" t="n">
         <v>701.5</v>
@@ -3130,12 +3130,12 @@
         <v>7.5</v>
       </c>
       <c r="E158" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28139</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28109</v>
       </c>
       <c r="B159" t="n">
         <v>702</v>
@@ -3147,12 +3147,12 @@
         <v>18</v>
       </c>
       <c r="E159" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28140</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28110</v>
       </c>
       <c r="B160" t="n">
         <v>692</v>
@@ -3164,12 +3164,12 @@
         <v>7</v>
       </c>
       <c r="E160" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28141</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28111</v>
       </c>
       <c r="B161" t="n">
         <v>690</v>
@@ -3181,12 +3181,12 @@
         <v>14</v>
       </c>
       <c r="E161" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28142</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28114</v>
       </c>
       <c r="B162" t="n">
         <v>684.5</v>
@@ -3198,12 +3198,12 @@
         <v>5</v>
       </c>
       <c r="E162" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28145</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28115</v>
       </c>
       <c r="B163" t="n">
         <v>688</v>
@@ -3215,12 +3215,12 @@
         <v>9</v>
       </c>
       <c r="E163" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28146</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28116</v>
       </c>
       <c r="B164" t="n">
         <v>693.5</v>
@@ -3232,12 +3232,12 @@
         <v>7</v>
       </c>
       <c r="E164" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28147</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28117</v>
       </c>
       <c r="B165" t="n">
         <v>693</v>
@@ -3249,12 +3249,12 @@
         <v>8.5</v>
       </c>
       <c r="E165" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28148</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28121</v>
       </c>
       <c r="B166" t="n">
         <v>705</v>
@@ -3266,12 +3266,12 @@
         <v>11</v>
       </c>
       <c r="E166" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28152</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28122</v>
       </c>
       <c r="B167" t="n">
         <v>706.5</v>
@@ -3283,12 +3283,12 @@
         <v>9</v>
       </c>
       <c r="E167" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28153</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28123</v>
       </c>
       <c r="B168" t="n">
         <v>710</v>
@@ -3300,12 +3300,12 @@
         <v>11</v>
       </c>
       <c r="E168" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28154</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
-        <v>25569.00000022872</v>
+        <v>28124</v>
       </c>
       <c r="B169" t="n">
         <v>708</v>
@@ -3317,12 +3317,12 @@
         <v>10</v>
       </c>
       <c r="E169" s="2" t="n">
-        <v>25600.00000022872</v>
+        <v>28155</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28128</v>
       </c>
       <c r="B170" t="n">
         <v>712</v>
@@ -3334,12 +3334,12 @@
         <v>14</v>
       </c>
       <c r="E170" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28159</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28129</v>
       </c>
       <c r="B171" t="n">
         <v>706</v>
@@ -3351,12 +3351,12 @@
         <v>14</v>
       </c>
       <c r="E171" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28160</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28130</v>
       </c>
       <c r="B172" t="n">
         <v>708</v>
@@ -3368,12 +3368,12 @@
         <v>7.75</v>
       </c>
       <c r="E172" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28161</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28131</v>
       </c>
       <c r="B173" t="n">
         <v>713.88</v>
@@ -3385,12 +3385,12 @@
         <v>13.88</v>
       </c>
       <c r="E173" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28162</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28132</v>
       </c>
       <c r="B174" t="n">
         <v>714</v>
@@ -3402,12 +3402,12 @@
         <v>5.5</v>
       </c>
       <c r="E174" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28163</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28135</v>
       </c>
       <c r="B175" t="n">
         <v>721.5</v>
@@ -3419,12 +3419,12 @@
         <v>6.5</v>
       </c>
       <c r="E175" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28166</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28136</v>
       </c>
       <c r="B176" t="n">
         <v>717</v>
@@ -3436,12 +3436,12 @@
         <v>7</v>
       </c>
       <c r="E176" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28167</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28137</v>
       </c>
       <c r="B177" t="n">
         <v>721</v>
@@ -3453,12 +3453,12 @@
         <v>9</v>
       </c>
       <c r="E177" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28168</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28138</v>
       </c>
       <c r="B178" t="n">
         <v>720</v>
@@ -3470,12 +3470,12 @@
         <v>9.75</v>
       </c>
       <c r="E178" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28169</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28139</v>
       </c>
       <c r="B179" t="n">
         <v>714.5</v>
@@ -3487,12 +3487,12 @@
         <v>8.5</v>
       </c>
       <c r="E179" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28170</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28142</v>
       </c>
       <c r="B180" t="n">
         <v>712</v>
@@ -3504,12 +3504,12 @@
         <v>4</v>
       </c>
       <c r="E180" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28173</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28143</v>
       </c>
       <c r="B181" t="n">
         <v>722.5</v>
@@ -3521,12 +3521,12 @@
         <v>12.5</v>
       </c>
       <c r="E181" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28174</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28144</v>
       </c>
       <c r="B182" t="n">
         <v>727.5</v>
@@ -3538,12 +3538,12 @@
         <v>7.5</v>
       </c>
       <c r="E182" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28175</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28145</v>
       </c>
       <c r="B183" t="n">
         <v>729.5</v>
@@ -3555,12 +3555,12 @@
         <v>10</v>
       </c>
       <c r="E183" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28176</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28146</v>
       </c>
       <c r="B184" t="n">
         <v>726</v>
@@ -3572,12 +3572,12 @@
         <v>6</v>
       </c>
       <c r="E184" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28177</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28149</v>
       </c>
       <c r="B185" t="n">
         <v>738</v>
@@ -3589,12 +3589,12 @@
         <v>17.5</v>
       </c>
       <c r="E185" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28180</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28150</v>
       </c>
       <c r="B186" t="n">
         <v>737</v>
@@ -3606,12 +3606,12 @@
         <v>5.75</v>
       </c>
       <c r="E186" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28181</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28151</v>
       </c>
       <c r="B187" t="n">
         <v>738</v>
@@ -3623,12 +3623,12 @@
         <v>15.5</v>
       </c>
       <c r="E187" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28182</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28152</v>
       </c>
       <c r="B188" t="n">
         <v>737</v>
@@ -3640,12 +3640,12 @@
         <v>20</v>
       </c>
       <c r="E188" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28183</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28153</v>
       </c>
       <c r="B189" t="n">
         <v>725.5</v>
@@ -3657,12 +3657,12 @@
         <v>12.5</v>
       </c>
       <c r="E189" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28184</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28156</v>
       </c>
       <c r="B190" t="n">
         <v>724.5</v>
@@ -3674,12 +3674,12 @@
         <v>8</v>
       </c>
       <c r="E190" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28184</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28157</v>
       </c>
       <c r="B191" t="n">
         <v>724</v>
@@ -3691,12 +3691,12 @@
         <v>8</v>
       </c>
       <c r="E191" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28185</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28158</v>
       </c>
       <c r="B192" t="n">
         <v>720.5</v>
@@ -3708,12 +3708,12 @@
         <v>5.5</v>
       </c>
       <c r="E192" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28186</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28159</v>
       </c>
       <c r="B193" t="n">
         <v>735.5</v>
@@ -3725,12 +3725,12 @@
         <v>13.5</v>
       </c>
       <c r="E193" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28187</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28160</v>
       </c>
       <c r="B194" t="n">
         <v>733</v>
@@ -3742,12 +3742,12 @@
         <v>7</v>
       </c>
       <c r="E194" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28188</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28163</v>
       </c>
       <c r="B195" t="n">
         <v>741.5</v>
@@ -3759,12 +3759,12 @@
         <v>12.5</v>
       </c>
       <c r="E195" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28191</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28164</v>
       </c>
       <c r="B196" t="n">
         <v>735</v>
@@ -3776,12 +3776,12 @@
         <v>10</v>
       </c>
       <c r="E196" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28192</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28165</v>
       </c>
       <c r="B197" t="n">
         <v>737.5</v>
@@ -3793,12 +3793,12 @@
         <v>7</v>
       </c>
       <c r="E197" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28193</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28166</v>
       </c>
       <c r="B198" t="n">
         <v>738</v>
@@ -3810,12 +3810,12 @@
         <v>5.5</v>
       </c>
       <c r="E198" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28194</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28167</v>
       </c>
       <c r="B199" t="n">
         <v>737.5</v>
@@ -3827,12 +3827,12 @@
         <v>4</v>
       </c>
       <c r="E199" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28195</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28170</v>
       </c>
       <c r="B200" t="n">
         <v>733</v>
@@ -3844,12 +3844,12 @@
         <v>3.5</v>
       </c>
       <c r="E200" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28198</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28171</v>
       </c>
       <c r="B201" t="n">
         <v>732.5</v>
@@ -3861,12 +3861,12 @@
         <v>6</v>
       </c>
       <c r="E201" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28199</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28172</v>
       </c>
       <c r="B202" t="n">
         <v>734.75</v>
@@ -3878,12 +3878,12 @@
         <v>9.25</v>
       </c>
       <c r="E202" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28200</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28173</v>
       </c>
       <c r="B203" t="n">
         <v>743.25</v>
@@ -3895,12 +3895,12 @@
         <v>8.25</v>
       </c>
       <c r="E203" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28201</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28174</v>
       </c>
       <c r="B204" t="n">
         <v>745.5</v>
@@ -3912,12 +3912,12 @@
         <v>6</v>
       </c>
       <c r="E204" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28202</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28178</v>
       </c>
       <c r="B205" t="n">
         <v>746</v>
@@ -3929,12 +3929,12 @@
         <v>4</v>
       </c>
       <c r="E205" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28206</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28179</v>
       </c>
       <c r="B206" t="n">
         <v>772</v>
@@ -3946,12 +3946,12 @@
         <v>26.5</v>
       </c>
       <c r="E206" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28207</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28180</v>
       </c>
       <c r="B207" t="n">
         <v>772</v>
@@ -3963,12 +3963,12 @@
         <v>11.5</v>
       </c>
       <c r="E207" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28208</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28181</v>
       </c>
       <c r="B208" t="n">
         <v>771</v>
@@ -3980,12 +3980,12 @@
         <v>12</v>
       </c>
       <c r="E208" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28209</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28184</v>
       </c>
       <c r="B209" t="n">
         <v>786.5</v>
@@ -3997,12 +3997,12 @@
         <v>19.5</v>
       </c>
       <c r="E209" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28212</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28185</v>
       </c>
       <c r="B210" t="n">
         <v>784.5</v>
@@ -4014,12 +4014,12 @@
         <v>13.5</v>
       </c>
       <c r="E210" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28216</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28186</v>
       </c>
       <c r="B211" t="n">
         <v>803</v>
@@ -4031,12 +4031,12 @@
         <v>15.5</v>
       </c>
       <c r="E211" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28217</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28187</v>
       </c>
       <c r="B212" t="n">
         <v>832</v>
@@ -4048,12 +4048,12 @@
         <v>29</v>
       </c>
       <c r="E212" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28218</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28188</v>
       </c>
       <c r="B213" t="n">
         <v>823</v>
@@ -4065,12 +4065,12 @@
         <v>8.5</v>
       </c>
       <c r="E213" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28219</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28191</v>
       </c>
       <c r="B214" t="n">
         <v>845</v>
@@ -4082,12 +4082,12 @@
         <v>22</v>
       </c>
       <c r="E214" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28222</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28192</v>
       </c>
       <c r="B215" t="n">
         <v>855</v>
@@ -4099,12 +4099,12 @@
         <v>31</v>
       </c>
       <c r="E215" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28223</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28193</v>
       </c>
       <c r="B216" t="n">
         <v>842</v>
@@ -4116,12 +4116,12 @@
         <v>21</v>
       </c>
       <c r="E216" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28224</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28194</v>
       </c>
       <c r="B217" t="n">
         <v>841.5</v>
@@ -4133,12 +4133,12 @@
         <v>31</v>
       </c>
       <c r="E217" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28225</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28195</v>
       </c>
       <c r="B218" t="n">
         <v>826.5</v>
@@ -4150,12 +4150,12 @@
         <v>22.5</v>
       </c>
       <c r="E218" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28226</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28198</v>
       </c>
       <c r="B219" t="n">
         <v>831</v>
@@ -4167,12 +4167,12 @@
         <v>17</v>
       </c>
       <c r="E219" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28229</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28199</v>
       </c>
       <c r="B220" t="n">
         <v>830.5</v>
@@ -4184,12 +4184,12 @@
         <v>9</v>
       </c>
       <c r="E220" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28230</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28200</v>
       </c>
       <c r="B221" t="n">
         <v>852</v>
@@ -4201,12 +4201,12 @@
         <v>17</v>
       </c>
       <c r="E221" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28231</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28201</v>
       </c>
       <c r="B222" t="n">
         <v>873.5</v>
@@ -4218,12 +4218,12 @@
         <v>28.5</v>
       </c>
       <c r="E222" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28232</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28202</v>
       </c>
       <c r="B223" t="n">
         <v>856</v>
@@ -4235,12 +4235,12 @@
         <v>14</v>
       </c>
       <c r="E223" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28233</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28205</v>
       </c>
       <c r="B224" t="n">
         <v>870</v>
@@ -4252,12 +4252,12 @@
         <v>15</v>
       </c>
       <c r="E224" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28236</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28206</v>
       </c>
       <c r="B225" t="n">
         <v>862</v>
@@ -4269,12 +4269,12 @@
         <v>10.5</v>
       </c>
       <c r="E225" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28237</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28207</v>
       </c>
       <c r="B226" t="n">
         <v>881</v>
@@ -4286,12 +4286,12 @@
         <v>35</v>
       </c>
       <c r="E226" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28238</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28208</v>
       </c>
       <c r="B227" t="n">
         <v>853</v>
@@ -4303,12 +4303,12 @@
         <v>12</v>
       </c>
       <c r="E227" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28239</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28209</v>
       </c>
       <c r="B228" t="n">
         <v>866</v>
@@ -4320,12 +4320,12 @@
         <v>22</v>
       </c>
       <c r="E228" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28240</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28212</v>
       </c>
       <c r="B229" t="n">
         <v>875</v>
@@ -4337,12 +4337,12 @@
         <v>18</v>
       </c>
       <c r="E229" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28243</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28213</v>
       </c>
       <c r="B230" t="n">
         <v>890</v>
@@ -4354,12 +4354,12 @@
         <v>23</v>
       </c>
       <c r="E230" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28244</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28214</v>
       </c>
       <c r="B231" t="n">
         <v>899</v>
@@ -4371,12 +4371,12 @@
         <v>13.5</v>
       </c>
       <c r="E231" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28245</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28215</v>
       </c>
       <c r="B232" t="n">
         <v>895</v>
@@ -4388,12 +4388,12 @@
         <v>13.5</v>
       </c>
       <c r="E232" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28245</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28216</v>
       </c>
       <c r="B233" t="n">
         <v>923</v>
@@ -4405,12 +4405,12 @@
         <v>15</v>
       </c>
       <c r="E233" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28246</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28219</v>
       </c>
       <c r="B234" t="n">
         <v>927</v>
@@ -4422,12 +4422,12 @@
         <v>13</v>
       </c>
       <c r="E234" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28249</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28220</v>
       </c>
       <c r="B235" t="n">
         <v>948</v>
@@ -4439,12 +4439,12 @@
         <v>15</v>
       </c>
       <c r="E235" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28250</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28221</v>
       </c>
       <c r="B236" t="n">
         <v>959</v>
@@ -4456,12 +4456,12 @@
         <v>19</v>
       </c>
       <c r="E236" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28251</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28222</v>
       </c>
       <c r="B237" t="n">
         <v>974</v>
@@ -4473,12 +4473,12 @@
         <v>25</v>
       </c>
       <c r="E237" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28252</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28226</v>
       </c>
       <c r="B238" t="n">
         <v>995</v>
@@ -4490,12 +4490,12 @@
         <v>25</v>
       </c>
       <c r="E238" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28256</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28227</v>
       </c>
       <c r="B239" t="n">
         <v>1023.5</v>
@@ -4507,12 +4507,12 @@
         <v>29.5</v>
       </c>
       <c r="E239" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28257</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="2" t="n">
-        <v>25569.00000022882</v>
+        <v>28228</v>
       </c>
       <c r="B240" t="n">
         <v>1053.5</v>
@@ -4524,7 +4524,7 @@
         <v>60</v>
       </c>
       <c r="E240" s="2" t="n">
-        <v>25600.00000022882</v>
+        <v>28258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>